<commit_message>
Removed references SDGR articles
Removed the references to the SDGR above article 12
</commit_message>
<xml_diff>
--- a/SDG concepts/SDG concepts_v0.01.xlsx
+++ b/SDG concepts/SDG concepts_v0.01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pittomvm\Documents\2 - Projects\Catalogue of Services\phase 7\D03.01\DG GROW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7AADF94-B63A-4BB6-A405-F48991BD22B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C0A0251E-5067-4A12-8387-5D7E62E174FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3435" yWindow="1275" windowWidth="28935" windowHeight="14010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11850" yWindow="1230" windowWidth="27930" windowHeight="13695" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="223">
   <si>
     <t>Data modelling exercise for capturing the information requirements of the SDGR (art 9,10,11)</t>
   </si>
@@ -502,9 +502,6 @@
     <t>Language</t>
   </si>
   <si>
-    <t>Art. 9, 10, 11, 13</t>
-  </si>
-  <si>
     <t>"Any additional languages in which the procedure can be carried out."
 "Member States will make the information accessible in an official language of the Union that is broadly understood by the largest possible number of cross-border users, in accordance with Article 12;"
 The language in which the service can be provided may differ from the language of certain channels (e.g. Web Pages in several languages vs provision of the service in 1-2 languages)</t>
@@ -676,9 +673,6 @@
     <t>Web Page</t>
   </si>
   <si>
-    <t>Art. 2, 5, 7, 9, 17, 18, 19</t>
-  </si>
-  <si>
     <t xml:space="preserve">The webpages on which the required information of Annex I and II will be posted. </t>
   </si>
   <si>
@@ -698,9 +692,6 @@
   </si>
   <si>
     <t>Type of channel</t>
-  </si>
-  <si>
-    <t>Art. 9, 11, 13</t>
   </si>
   <si>
     <t>Code list for all the different media which can be used to access information about or request a service: Phone, Email, Web Page, Online Enquiry Form etc.</t>
@@ -893,9 +884,6 @@
     <t>Procedure</t>
   </si>
   <si>
-    <t>Art. 3, 10, 13, 14</t>
-  </si>
-  <si>
     <t>"A sequence of actions that must be taken by users to satisfy the requirements, or to obtain from a competent authority a decision, in order to be able to exercise their rights as referred to in point (a) of Article 2(2);"</t>
   </si>
   <si>
@@ -956,9 +944,6 @@
     <t>Deadline</t>
   </si>
   <si>
-    <t>Art. 10, 11, 13, 16</t>
-  </si>
-  <si>
     <t>"(g) any deadlines to be respected by the user or by the competent authority"
 Period of time, linked to a date (own interpretation)
  When deadlines are extended, users are informed in advance of the reasons thereof and of the new deadline given</t>
@@ -968,9 +953,6 @@
   </si>
   <si>
     <t>Average/estimated time</t>
-  </si>
-  <si>
-    <t>Art. 10, 11, 13</t>
   </si>
   <si>
     <t>"where no deadlines exist, the average, estimated or indicative time that the competent authority needs to complete the procedure"</t>
@@ -1010,9 +992,6 @@
   </si>
   <si>
     <t>Evidence</t>
-  </si>
-  <si>
-    <t>Art. 3, 6, 13, 14</t>
   </si>
   <si>
     <t>"Any document or data, including text or sound, visual or audiovisual recording, irrespective of the medium used, required by a competent authority to prove facts or compliance with procedural requirements referred to in point (b) of Article 2(2)."</t>
@@ -1082,9 +1061,6 @@
   </si>
   <si>
     <t>Requirement</t>
-  </si>
-  <si>
-    <t>Art. 3, 6, 13</t>
   </si>
   <si>
     <t>"users to fulfil the requirements related to the procedure in a user-friendly and structured way"
@@ -1520,9 +1496,6 @@
     <t>Authentication</t>
   </si>
   <si>
-    <t>Art. 10, 13, 15</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="10"/>
@@ -1553,9 +1526,6 @@
     <t>Identification</t>
   </si>
   <si>
-    <t>Art. 6, 10, 13</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="10"/>
@@ -1581,9 +1551,6 @@
       </rPr>
       <t>and signature for the procedure;</t>
     </r>
-  </si>
-  <si>
-    <t>Art. 10, 13</t>
   </si>
   <si>
     <r>
@@ -1644,6 +1611,21 @@
   </si>
   <si>
     <t>I don't know</t>
+  </si>
+  <si>
+    <t>Art. 3, 10</t>
+  </si>
+  <si>
+    <t>Art. 10, 11</t>
+  </si>
+  <si>
+    <t>Art. 3, 6</t>
+  </si>
+  <si>
+    <t>Art. 6, 10</t>
+  </si>
+  <si>
+    <t>Art. 2, 5, 7, 9</t>
   </si>
 </sst>
 </file>
@@ -2066,12 +2048,19 @@
     <xf numFmtId="0" fontId="22" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -2084,21 +2073,14 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2321,7 +2303,7 @@
   </sheetPr>
   <dimension ref="B1:K47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A19" workbookViewId="0">
       <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
@@ -2347,15 +2329,15 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:11" ht="27.75" customHeight="1">
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
@@ -2387,15 +2369,15 @@
       <c r="K4" s="3"/>
     </row>
     <row r="5" spans="2:11" ht="186.6" customHeight="1">
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
-      <c r="G5" s="48"/>
-      <c r="H5" s="48"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
+      <c r="F5" s="51"/>
+      <c r="G5" s="51"/>
+      <c r="H5" s="51"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
@@ -2418,7 +2400,7 @@
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
-      <c r="E7" s="56" t="s">
+      <c r="E7" s="46" t="s">
         <v>4</v>
       </c>
       <c r="F7" s="3"/>
@@ -2441,15 +2423,15 @@
       <c r="K8" s="3"/>
     </row>
     <row r="9" spans="2:11" ht="12.75">
-      <c r="B9" s="52" t="s">
+      <c r="B9" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="48"/>
-      <c r="D9" s="48"/>
-      <c r="E9" s="48"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="48"/>
-      <c r="H9" s="48"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
+      <c r="F9" s="51"/>
+      <c r="G9" s="51"/>
+      <c r="H9" s="51"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
@@ -2493,15 +2475,15 @@
       <c r="K12" s="3"/>
     </row>
     <row r="13" spans="2:11" ht="32.1" customHeight="1">
-      <c r="B13" s="52" t="s">
+      <c r="B13" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="48"/>
-      <c r="D13" s="48"/>
-      <c r="E13" s="48"/>
-      <c r="F13" s="48"/>
-      <c r="G13" s="48"/>
-      <c r="H13" s="48"/>
+      <c r="C13" s="51"/>
+      <c r="D13" s="51"/>
+      <c r="E13" s="51"/>
+      <c r="F13" s="51"/>
+      <c r="G13" s="51"/>
+      <c r="H13" s="51"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
@@ -2585,7 +2567,7 @@
         <v>15</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -2831,17 +2813,17 @@
       <c r="K35" s="40"/>
     </row>
     <row r="36" spans="2:11" ht="43.5" customHeight="1">
-      <c r="B36" s="44" t="s">
+      <c r="B36" s="56" t="s">
         <v>34</v>
       </c>
-      <c r="C36" s="45"/>
-      <c r="D36" s="46"/>
-      <c r="E36" s="49" t="s">
+      <c r="C36" s="48"/>
+      <c r="D36" s="49"/>
+      <c r="E36" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="F36" s="50"/>
-      <c r="G36" s="50"/>
-      <c r="H36" s="51"/>
+      <c r="F36" s="53"/>
+      <c r="G36" s="53"/>
+      <c r="H36" s="54"/>
       <c r="I36" s="15" t="s">
         <v>36</v>
       </c>
@@ -2849,17 +2831,17 @@
       <c r="K36" s="3"/>
     </row>
     <row r="37" spans="2:11" ht="43.5" customHeight="1">
-      <c r="B37" s="57" t="s">
+      <c r="B37" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="C37" s="45"/>
-      <c r="D37" s="46"/>
-      <c r="E37" s="49" t="s">
+      <c r="C37" s="48"/>
+      <c r="D37" s="49"/>
+      <c r="E37" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="F37" s="50"/>
-      <c r="G37" s="50"/>
-      <c r="H37" s="51"/>
+      <c r="F37" s="53"/>
+      <c r="G37" s="53"/>
+      <c r="H37" s="54"/>
       <c r="I37" s="15" t="s">
         <v>38</v>
       </c>
@@ -2867,17 +2849,17 @@
       <c r="K37" s="3"/>
     </row>
     <row r="38" spans="2:11" ht="43.5" customHeight="1">
-      <c r="B38" s="44" t="s">
+      <c r="B38" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="C38" s="45"/>
-      <c r="D38" s="46"/>
-      <c r="E38" s="49" t="s">
+      <c r="C38" s="48"/>
+      <c r="D38" s="49"/>
+      <c r="E38" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="F38" s="50"/>
-      <c r="G38" s="50"/>
-      <c r="H38" s="51"/>
+      <c r="F38" s="53"/>
+      <c r="G38" s="53"/>
+      <c r="H38" s="54"/>
       <c r="I38" s="15" t="s">
         <v>38</v>
       </c>
@@ -2885,17 +2867,17 @@
       <c r="K38" s="3"/>
     </row>
     <row r="39" spans="2:11" ht="43.5" customHeight="1">
-      <c r="B39" s="44" t="s">
+      <c r="B39" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="C39" s="45"/>
-      <c r="D39" s="46"/>
-      <c r="E39" s="49" t="s">
+      <c r="C39" s="48"/>
+      <c r="D39" s="49"/>
+      <c r="E39" s="52" t="s">
         <v>42</v>
       </c>
-      <c r="F39" s="50"/>
-      <c r="G39" s="50"/>
-      <c r="H39" s="51"/>
+      <c r="F39" s="53"/>
+      <c r="G39" s="53"/>
+      <c r="H39" s="54"/>
       <c r="I39" s="15" t="s">
         <v>38</v>
       </c>
@@ -2915,17 +2897,17 @@
       <c r="K40" s="3"/>
     </row>
     <row r="41" spans="2:11" ht="28.5" customHeight="1">
-      <c r="B41" s="47" t="s">
+      <c r="B41" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="C41" s="48"/>
-      <c r="D41" s="48"/>
-      <c r="E41" s="48"/>
-      <c r="F41" s="48"/>
-      <c r="G41" s="48"/>
-      <c r="H41" s="48"/>
-      <c r="I41" s="48"/>
-      <c r="J41" s="48"/>
+      <c r="C41" s="51"/>
+      <c r="D41" s="51"/>
+      <c r="E41" s="51"/>
+      <c r="F41" s="51"/>
+      <c r="G41" s="51"/>
+      <c r="H41" s="51"/>
+      <c r="I41" s="51"/>
+      <c r="J41" s="51"/>
       <c r="K41" s="3"/>
     </row>
     <row r="42" spans="2:11" ht="12.75">
@@ -3006,6 +2988,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="B41:J41"/>
+    <mergeCell ref="E38:H38"/>
+    <mergeCell ref="E39:H39"/>
     <mergeCell ref="B37:D37"/>
     <mergeCell ref="B13:H13"/>
     <mergeCell ref="E36:H36"/>
@@ -3014,11 +3001,6 @@
     <mergeCell ref="B5:H5"/>
     <mergeCell ref="B9:H9"/>
     <mergeCell ref="B36:D36"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="B41:J41"/>
-    <mergeCell ref="E38:H38"/>
-    <mergeCell ref="E39:H39"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E7" location="'1 - Concepts SDG'!A1" display="1 - Concepts SDG" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -3035,11 +3017,11 @@
   </sheetPr>
   <dimension ref="A1:AB976"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomRight" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -3273,16 +3255,16 @@
         <v>73</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>74</v>
+        <v>115</v>
       </c>
       <c r="C6" s="24" t="s">
         <v>23</v>
       </c>
       <c r="D6" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="E6" s="27" t="s">
         <v>75</v>
-      </c>
-      <c r="E6" s="27" t="s">
-        <v>76</v>
       </c>
       <c r="F6" s="28"/>
       <c r="G6" s="28"/>
@@ -3310,7 +3292,7 @@
     </row>
     <row r="7" spans="1:28" ht="25.5">
       <c r="A7" s="24" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B7" s="26" t="s">
         <v>57</v>
@@ -3319,10 +3301,10 @@
         <v>27</v>
       </c>
       <c r="D7" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="E7" s="27" t="s">
         <v>78</v>
-      </c>
-      <c r="E7" s="27" t="s">
-        <v>79</v>
       </c>
       <c r="F7" s="28"/>
       <c r="G7" s="28"/>
@@ -3360,7 +3342,7 @@
       </c>
       <c r="D8" s="25"/>
       <c r="E8" s="27" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F8" s="28"/>
       <c r="G8" s="28"/>
@@ -3388,19 +3370,19 @@
     </row>
     <row r="9" spans="1:28" ht="25.5">
       <c r="A9" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" s="26" t="s">
         <v>81</v>
-      </c>
-      <c r="B9" s="26" t="s">
-        <v>82</v>
       </c>
       <c r="C9" s="24" t="s">
         <v>27</v>
       </c>
       <c r="D9" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="E9" s="27" t="s">
         <v>83</v>
-      </c>
-      <c r="E9" s="27" t="s">
-        <v>84</v>
       </c>
       <c r="F9" s="28"/>
       <c r="G9" s="28"/>
@@ -3428,19 +3410,19 @@
     </row>
     <row r="10" spans="1:28" ht="25.5">
       <c r="A10" s="24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C10" s="24" t="s">
         <v>27</v>
       </c>
       <c r="D10" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="E10" s="27" t="s">
         <v>86</v>
-      </c>
-      <c r="E10" s="27" t="s">
-        <v>87</v>
       </c>
       <c r="F10" s="28"/>
       <c r="G10" s="28"/>
@@ -3468,7 +3450,7 @@
     </row>
     <row r="11" spans="1:28" ht="25.5">
       <c r="A11" s="24" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B11" s="26" t="s">
         <v>57</v>
@@ -3477,10 +3459,10 @@
         <v>25</v>
       </c>
       <c r="D11" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="E11" s="27" t="s">
         <v>89</v>
-      </c>
-      <c r="E11" s="27" t="s">
-        <v>90</v>
       </c>
       <c r="F11" s="28"/>
       <c r="G11" s="28"/>
@@ -3508,19 +3490,19 @@
     </row>
     <row r="12" spans="1:28" ht="63.75">
       <c r="A12" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="B12" s="26" t="s">
         <v>91</v>
-      </c>
-      <c r="B12" s="26" t="s">
-        <v>92</v>
       </c>
       <c r="C12" s="24" t="s">
         <v>25</v>
       </c>
       <c r="D12" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="E12" s="27" t="s">
         <v>93</v>
-      </c>
-      <c r="E12" s="27" t="s">
-        <v>94</v>
       </c>
       <c r="F12" s="28"/>
       <c r="G12" s="28"/>
@@ -3546,21 +3528,21 @@
       <c r="AA12" s="23"/>
       <c r="AB12" s="23"/>
     </row>
-    <row r="13" spans="1:28" ht="25.5">
+    <row r="13" spans="1:28" ht="12.75">
       <c r="A13" s="24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>96</v>
+        <v>222</v>
       </c>
       <c r="C13" s="24" t="s">
         <v>23</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E13" s="25" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F13" s="28"/>
       <c r="G13" s="28"/>
@@ -3588,25 +3570,25 @@
     </row>
     <row r="14" spans="1:28" ht="25.5">
       <c r="A14" s="24" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>74</v>
+        <v>115</v>
       </c>
       <c r="C14" s="24" t="s">
         <v>23</v>
       </c>
       <c r="D14" s="25" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E14" s="25" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F14" s="28"/>
       <c r="G14" s="28"/>
       <c r="H14" s="28"/>
       <c r="I14" s="25" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J14" s="28"/>
       <c r="K14" s="23"/>
@@ -3630,23 +3612,23 @@
     </row>
     <row r="15" spans="1:28" ht="38.25">
       <c r="A15" s="24" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B15" s="26" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C15" s="24" t="s">
         <v>25</v>
       </c>
       <c r="D15" s="25"/>
       <c r="E15" s="25" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F15" s="28"/>
       <c r="G15" s="28"/>
       <c r="H15" s="28"/>
       <c r="I15" s="25" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="J15" s="28"/>
       <c r="K15" s="23"/>
@@ -3670,25 +3652,25 @@
     </row>
     <row r="16" spans="1:28" ht="140.25">
       <c r="A16" s="24" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C16" s="24" t="s">
         <v>23</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E16" s="25" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F16" s="28"/>
       <c r="G16" s="28"/>
       <c r="H16" s="28"/>
       <c r="I16" s="25" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="J16" s="28"/>
       <c r="K16" s="23"/>
@@ -3712,16 +3694,16 @@
     </row>
     <row r="17" spans="1:28" ht="12.75">
       <c r="A17" s="24" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B17" s="26" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C17" s="24" t="s">
         <v>23</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E17" s="25"/>
       <c r="F17" s="28"/>
@@ -3750,16 +3732,16 @@
     </row>
     <row r="18" spans="1:28" ht="25.5">
       <c r="A18" s="24" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C18" s="24" t="s">
         <v>25</v>
       </c>
       <c r="D18" s="25" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E18" s="25" t="s">
         <v>64</v>
@@ -3790,25 +3772,25 @@
     </row>
     <row r="19" spans="1:28" ht="114.75">
       <c r="A19" s="24" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B19" s="26" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C19" s="24" t="s">
         <v>23</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E19" s="27" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F19" s="28"/>
       <c r="G19" s="28"/>
       <c r="H19" s="28"/>
       <c r="I19" s="25" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="J19" s="28"/>
       <c r="K19" s="23"/>
@@ -3832,19 +3814,19 @@
     </row>
     <row r="20" spans="1:28" ht="25.5">
       <c r="A20" s="24" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C20" s="24" t="s">
         <v>27</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E20" s="25" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F20" s="28"/>
       <c r="G20" s="28"/>
@@ -3872,19 +3854,19 @@
     </row>
     <row r="21" spans="1:28" ht="25.5">
       <c r="A21" s="24" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B21" s="26" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C21" s="24" t="s">
         <v>27</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E21" s="25" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F21" s="28"/>
       <c r="G21" s="28"/>
@@ -3912,19 +3894,19 @@
     </row>
     <row r="22" spans="1:28" ht="25.5">
       <c r="A22" s="24" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C22" s="24" t="s">
         <v>27</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E22" s="25" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F22" s="28"/>
       <c r="G22" s="28"/>
@@ -3952,28 +3934,28 @@
     </row>
     <row r="23" spans="1:28" ht="63.75">
       <c r="A23" s="24" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B23" s="26" t="s">
-        <v>131</v>
+        <v>218</v>
       </c>
       <c r="C23" s="24" t="s">
         <v>23</v>
       </c>
       <c r="D23" s="25" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="E23" s="25" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="F23" s="28"/>
       <c r="G23" s="28"/>
       <c r="H23" s="28"/>
       <c r="I23" s="25" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="J23" s="28" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="K23" s="23"/>
       <c r="L23" s="23"/>
@@ -3996,19 +3978,19 @@
     </row>
     <row r="24" spans="1:28" ht="38.25">
       <c r="A24" s="24" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B24" s="26" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C24" s="24" t="s">
         <v>23</v>
       </c>
       <c r="D24" s="25" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="E24" s="25" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="F24" s="28"/>
       <c r="G24" s="28"/>
@@ -4036,19 +4018,19 @@
     </row>
     <row r="25" spans="1:28" ht="38.25">
       <c r="A25" s="24" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="B25" s="26" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C25" s="24" t="s">
         <v>25</v>
       </c>
       <c r="D25" s="25" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E25" s="25" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F25" s="28"/>
       <c r="G25" s="28"/>
@@ -4076,19 +4058,19 @@
     </row>
     <row r="26" spans="1:28" ht="51">
       <c r="A26" s="24" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B26" s="26" t="s">
-        <v>144</v>
+        <v>219</v>
       </c>
       <c r="C26" s="24" t="s">
         <v>27</v>
       </c>
       <c r="D26" s="25" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="E26" s="25" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="F26" s="28"/>
       <c r="G26" s="28"/>
@@ -4116,19 +4098,19 @@
     </row>
     <row r="27" spans="1:28" ht="25.5">
       <c r="A27" s="24" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>148</v>
+        <v>219</v>
       </c>
       <c r="C27" s="24" t="s">
         <v>27</v>
       </c>
       <c r="D27" s="25" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="E27" s="25" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="F27" s="28"/>
       <c r="G27" s="28"/>
@@ -4156,16 +4138,16 @@
     </row>
     <row r="28" spans="1:28" ht="38.25">
       <c r="A28" s="24" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="B28" s="26" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C28" s="24" t="s">
         <v>27</v>
       </c>
       <c r="D28" s="25" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="E28" s="25"/>
       <c r="F28" s="28"/>
@@ -4194,19 +4176,19 @@
     </row>
     <row r="29" spans="1:28" ht="38.25">
       <c r="A29" s="24" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B29" s="26" t="s">
-        <v>154</v>
+        <v>220</v>
       </c>
       <c r="C29" s="24" t="s">
         <v>23</v>
       </c>
       <c r="D29" s="25" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="E29" s="27" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="F29" s="28"/>
       <c r="G29" s="28"/>
@@ -4234,16 +4216,16 @@
     </row>
     <row r="30" spans="1:28" ht="12.75">
       <c r="A30" s="24" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B30" s="26" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C30" s="24" t="s">
         <v>23</v>
       </c>
       <c r="D30" s="25" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="E30" s="25"/>
       <c r="F30" s="28"/>
@@ -4272,16 +4254,16 @@
     </row>
     <row r="31" spans="1:28" ht="12.75">
       <c r="A31" s="24" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="B31" s="26" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C31" s="24" t="s">
         <v>27</v>
       </c>
       <c r="D31" s="25" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="E31" s="25"/>
       <c r="F31" s="28"/>
@@ -4310,16 +4292,16 @@
     </row>
     <row r="32" spans="1:28" ht="76.5">
       <c r="A32" s="24" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="B32" s="26" t="s">
-        <v>162</v>
+        <v>220</v>
       </c>
       <c r="C32" s="24" t="s">
         <v>25</v>
       </c>
       <c r="D32" s="25" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="E32" s="25"/>
       <c r="F32" s="28"/>
@@ -4348,19 +4330,19 @@
     </row>
     <row r="33" spans="1:28" ht="25.5">
       <c r="A33" s="24" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B33" s="26" t="s">
-        <v>144</v>
+        <v>219</v>
       </c>
       <c r="C33" s="24" t="s">
         <v>25</v>
       </c>
       <c r="D33" s="25" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="E33" s="25" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="F33" s="28"/>
       <c r="G33" s="28"/>
@@ -4388,25 +4370,25 @@
     </row>
     <row r="34" spans="1:28" ht="38.25">
       <c r="A34" s="24" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="B34" s="26" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="C34" s="24" t="s">
         <v>27</v>
       </c>
       <c r="D34" s="25" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="E34" s="25" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="F34" s="28"/>
       <c r="G34" s="28"/>
       <c r="H34" s="28"/>
       <c r="I34" s="25" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="J34" s="28"/>
       <c r="K34" s="23"/>
@@ -4430,17 +4412,17 @@
     </row>
     <row r="35" spans="1:28" ht="25.5">
       <c r="A35" s="24" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="B35" s="26" t="s">
-        <v>144</v>
+        <v>219</v>
       </c>
       <c r="C35" s="24" t="s">
         <v>25</v>
       </c>
       <c r="D35" s="25"/>
       <c r="E35" s="25" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="F35" s="28"/>
       <c r="G35" s="28"/>
@@ -4468,23 +4450,23 @@
     </row>
     <row r="36" spans="1:28" ht="25.5">
       <c r="A36" s="24" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="B36" s="26" t="s">
-        <v>144</v>
+        <v>219</v>
       </c>
       <c r="C36" s="24" t="s">
         <v>25</v>
       </c>
       <c r="D36" s="25" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="E36" s="25"/>
       <c r="F36" s="28"/>
       <c r="G36" s="28"/>
       <c r="H36" s="28"/>
       <c r="I36" s="25" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="J36" s="28"/>
       <c r="K36" s="23"/>
@@ -4508,19 +4490,19 @@
     </row>
     <row r="37" spans="1:28" ht="25.5">
       <c r="A37" s="24" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="B37" s="26" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="C37" s="24" t="s">
         <v>23</v>
       </c>
       <c r="D37" s="25" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="E37" s="25" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="F37" s="28"/>
       <c r="G37" s="28"/>
@@ -4548,25 +4530,25 @@
     </row>
     <row r="38" spans="1:28" ht="76.5">
       <c r="A38" s="24" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="B38" s="26" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C38" s="24" t="s">
         <v>23</v>
       </c>
       <c r="D38" s="25" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="E38" s="25" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F38" s="28"/>
       <c r="G38" s="28"/>
       <c r="H38" s="28"/>
       <c r="I38" s="25" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="J38" s="28"/>
       <c r="K38" s="23"/>
@@ -4590,19 +4572,19 @@
     </row>
     <row r="39" spans="1:28" ht="114.75">
       <c r="A39" s="24" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="B39" s="26" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C39" s="24" t="s">
         <v>27</v>
       </c>
       <c r="D39" s="25" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="E39" s="25" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="F39" s="28"/>
       <c r="G39" s="28"/>
@@ -4630,16 +4612,16 @@
     </row>
     <row r="40" spans="1:28" ht="25.5">
       <c r="A40" s="24" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="B40" s="26" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C40" s="24" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="25" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="E40" s="25"/>
       <c r="F40" s="28"/>
@@ -4668,16 +4650,16 @@
     </row>
     <row r="41" spans="1:28" ht="25.5">
       <c r="A41" s="24" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="B41" s="26" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C41" s="24" t="s">
         <v>25</v>
       </c>
       <c r="D41" s="25" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="E41" s="25"/>
       <c r="F41" s="28"/>
@@ -4706,16 +4688,16 @@
     </row>
     <row r="42" spans="1:28" ht="25.5">
       <c r="A42" s="24" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="B42" s="26" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C42" s="24" t="s">
         <v>25</v>
       </c>
       <c r="D42" s="25" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="E42" s="25"/>
       <c r="F42" s="28"/>
@@ -4744,23 +4726,23 @@
     </row>
     <row r="43" spans="1:28" ht="25.5">
       <c r="A43" s="24" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="B43" s="26" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C43" s="24" t="s">
         <v>25</v>
       </c>
       <c r="D43" s="25" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="E43" s="25"/>
       <c r="F43" s="28"/>
       <c r="G43" s="28"/>
       <c r="H43" s="28"/>
       <c r="I43" s="25" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="J43" s="28"/>
       <c r="K43" s="23"/>
@@ -4784,23 +4766,23 @@
     </row>
     <row r="44" spans="1:28" ht="25.5">
       <c r="A44" s="24" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="B44" s="26" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C44" s="24" t="s">
         <v>25</v>
       </c>
       <c r="D44" s="25" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="E44" s="25"/>
       <c r="F44" s="28"/>
       <c r="G44" s="28"/>
       <c r="H44" s="28"/>
       <c r="I44" s="25" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="J44" s="28"/>
       <c r="K44" s="23"/>
@@ -4824,23 +4806,23 @@
     </row>
     <row r="45" spans="1:28" ht="51">
       <c r="A45" s="24" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="B45" s="26" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C45" s="24" t="s">
         <v>25</v>
       </c>
       <c r="D45" s="25" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="E45" s="25"/>
       <c r="F45" s="28"/>
       <c r="G45" s="28"/>
       <c r="H45" s="28"/>
       <c r="I45" s="25" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="J45" s="28"/>
       <c r="K45" s="23"/>
@@ -4864,23 +4846,23 @@
     </row>
     <row r="46" spans="1:28" ht="38.25">
       <c r="A46" s="24" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="B46" s="26" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C46" s="24" t="s">
         <v>25</v>
       </c>
       <c r="D46" s="25" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="E46" s="25"/>
       <c r="F46" s="28"/>
       <c r="G46" s="28"/>
       <c r="H46" s="28"/>
       <c r="I46" s="25" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="J46" s="28"/>
       <c r="K46" s="23"/>
@@ -4904,23 +4886,23 @@
     </row>
     <row r="47" spans="1:28" ht="38.25">
       <c r="A47" s="24" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="B47" s="26" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C47" s="24" t="s">
         <v>25</v>
       </c>
       <c r="D47" s="25" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="E47" s="25"/>
       <c r="F47" s="28"/>
       <c r="G47" s="28"/>
       <c r="H47" s="28"/>
       <c r="I47" s="25" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="J47" s="28"/>
       <c r="K47" s="23"/>
@@ -4944,23 +4926,23 @@
     </row>
     <row r="48" spans="1:28" ht="38.25">
       <c r="A48" s="24" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="B48" s="26" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C48" s="24" t="s">
         <v>25</v>
       </c>
       <c r="D48" s="25" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="E48" s="25"/>
       <c r="F48" s="28"/>
       <c r="G48" s="28"/>
       <c r="H48" s="28"/>
       <c r="I48" s="25" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="J48" s="28"/>
       <c r="K48" s="23"/>
@@ -4984,23 +4966,23 @@
     </row>
     <row r="49" spans="1:28" ht="38.25">
       <c r="A49" s="24" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="B49" s="26" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C49" s="24" t="s">
         <v>25</v>
       </c>
       <c r="D49" s="25" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="E49" s="25"/>
       <c r="F49" s="28"/>
       <c r="G49" s="28"/>
       <c r="H49" s="28"/>
       <c r="I49" s="25" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="J49" s="28"/>
       <c r="K49" s="23"/>
@@ -5024,23 +5006,23 @@
     </row>
     <row r="50" spans="1:28" ht="38.25">
       <c r="A50" s="24" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="B50" s="26" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C50" s="24" t="s">
         <v>25</v>
       </c>
       <c r="D50" s="25" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="E50" s="25"/>
       <c r="F50" s="28"/>
       <c r="G50" s="28"/>
       <c r="H50" s="28"/>
       <c r="I50" s="25" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="J50" s="28"/>
       <c r="K50" s="23"/>
@@ -5064,23 +5046,23 @@
     </row>
     <row r="51" spans="1:28" ht="25.5">
       <c r="A51" s="24" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="B51" s="26" t="s">
-        <v>211</v>
+        <v>133</v>
       </c>
       <c r="C51" s="24" t="s">
         <v>25</v>
       </c>
       <c r="D51" s="25" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="E51" s="25"/>
       <c r="F51" s="28"/>
       <c r="G51" s="28"/>
       <c r="H51" s="28"/>
       <c r="I51" s="25" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="J51" s="28"/>
       <c r="K51" s="23"/>
@@ -5104,23 +5086,23 @@
     </row>
     <row r="52" spans="1:28" ht="25.5">
       <c r="A52" s="24" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="B52" s="26" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="C52" s="24" t="s">
         <v>25</v>
       </c>
       <c r="D52" s="25" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="E52" s="25"/>
       <c r="F52" s="28"/>
       <c r="G52" s="28"/>
       <c r="H52" s="28"/>
       <c r="I52" s="25" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="J52" s="28"/>
       <c r="K52" s="23"/>
@@ -5144,23 +5126,23 @@
     </row>
     <row r="53" spans="1:28" ht="25.5">
       <c r="A53" s="24" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="B53" s="26" t="s">
-        <v>216</v>
+        <v>133</v>
       </c>
       <c r="C53" s="24" t="s">
         <v>25</v>
       </c>
       <c r="D53" s="25" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="E53" s="25"/>
       <c r="F53" s="28"/>
       <c r="G53" s="28"/>
       <c r="H53" s="28"/>
       <c r="I53" s="25" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="J53" s="28"/>
       <c r="K53" s="23"/>
@@ -5184,7 +5166,7 @@
     </row>
     <row r="54" spans="1:28" ht="24">
       <c r="A54" s="43" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="B54" s="31"/>
       <c r="C54" s="31"/>
@@ -5216,7 +5198,7 @@
     </row>
     <row r="55" spans="1:28" ht="24">
       <c r="A55" s="43" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="B55" s="31"/>
       <c r="C55" s="31"/>
@@ -5248,7 +5230,7 @@
     </row>
     <row r="56" spans="1:28" ht="24">
       <c r="A56" s="43" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="B56" s="31"/>
       <c r="C56" s="31"/>
@@ -5280,7 +5262,7 @@
     </row>
     <row r="57" spans="1:28" ht="24">
       <c r="A57" s="43" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="B57" s="31"/>
       <c r="C57" s="31"/>
@@ -5312,7 +5294,7 @@
     </row>
     <row r="58" spans="1:28" ht="24">
       <c r="A58" s="43" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="B58" s="31"/>
       <c r="C58" s="31"/>
@@ -5344,7 +5326,7 @@
     </row>
     <row r="59" spans="1:28" ht="24">
       <c r="A59" s="43" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="B59" s="31"/>
       <c r="C59" s="31"/>
@@ -5376,7 +5358,7 @@
     </row>
     <row r="60" spans="1:28" ht="24">
       <c r="A60" s="43" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="B60" s="31"/>
       <c r="C60" s="31"/>
@@ -5408,7 +5390,7 @@
     </row>
     <row r="61" spans="1:28" ht="24">
       <c r="A61" s="43" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="B61" s="31"/>
       <c r="C61" s="31"/>
@@ -32930,36 +32912,36 @@
     <col min="2" max="2" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="51.75" thickBot="1">
-      <c r="A1" s="54" t="s">
+    <row r="1" spans="1:2" ht="26.25" thickBot="1">
+      <c r="A1" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="54" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="26.25" thickBot="1">
-      <c r="A2" s="55" t="s">
-        <v>223</v>
-      </c>
-      <c r="B2" s="55" t="s">
-        <v>224</v>
+      <c r="B1" s="44" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="13.5" thickBot="1">
+      <c r="A2" s="45" t="s">
+        <v>212</v>
+      </c>
+      <c r="B2" s="45" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="13.5" thickBot="1">
-      <c r="A3" s="55" t="s">
-        <v>225</v>
-      </c>
-      <c r="B3" s="55" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="26.25" thickBot="1">
-      <c r="A4" s="55" t="s">
-        <v>227</v>
-      </c>
-      <c r="B4" s="55" t="s">
-        <v>228</v>
+      <c r="A3" s="45" t="s">
+        <v>214</v>
+      </c>
+      <c r="B3" s="45" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="13.5" thickBot="1">
+      <c r="A4" s="45" t="s">
+        <v>216</v>
+      </c>
+      <c r="B4" s="45" t="s">
+        <v>217</v>
       </c>
     </row>
   </sheetData>

</xml_diff>